<commit_message>
Fix onshore wind values in BPMCCS and PMCCS
</commit_message>
<xml_diff>
--- a/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us-analysis\InputData\elec\PMCCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\elec\PMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="61" r:id="rId6"/>
+    <pivotCache cacheId="19" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -30142,7 +30142,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="61" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField axis="axisCol" showAll="0">
@@ -92283,7 +92283,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2:AG17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -92801,25 +92801,25 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>20567.8</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>6732.8000000000011</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1946</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>895.5</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -94018,7 +94018,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -94673,31 +94673,31 @@
       </c>
       <c r="C6">
         <f>BPMCCS!C6</f>
-        <v>0</v>
+        <v>20567.8</v>
       </c>
       <c r="D6">
         <f>BPMCCS!D6</f>
-        <v>0</v>
+        <v>6732.8000000000011</v>
       </c>
       <c r="E6">
         <f>BPMCCS!E6</f>
-        <v>0</v>
+        <v>1946</v>
       </c>
       <c r="F6">
         <f>BPMCCS!F6</f>
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="G6">
         <f>BPMCCS!G6</f>
-        <v>0</v>
+        <v>895.5</v>
       </c>
       <c r="H6">
         <f>BPMCCS!H6</f>
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="I6">
         <f>BPMCCS!I6</f>
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="J6">
         <f>BPMCCS!J6</f>

</xml_diff>